<commit_message>
added progress updates field
</commit_message>
<xml_diff>
--- a/data/DummyData.xlsx
+++ b/data/DummyData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T71"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -452,16 +452,7 @@
         <v>Q4 Status</v>
       </c>
       <c r="Q1" t="str">
-        <v>Q1 Comments</v>
-      </c>
-      <c r="R1" t="str">
-        <v>Q2 Comments</v>
-      </c>
-      <c r="S1" t="str">
-        <v>Q3 Comments</v>
-      </c>
-      <c r="T1" t="str">
-        <v>Q4 Comments</v>
+        <v>Progress Updates</v>
       </c>
     </row>
     <row r="2">
@@ -531,7 +522,7 @@
         <v>missed</v>
       </c>
       <c r="N3" t="str">
-        <v>missed</v>
+        <v>on-track</v>
       </c>
       <c r="O3" t="str">
         <v>missed</v>
@@ -2526,7 +2517,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:T71"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q71"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Inline editing working for Progress updates, Q's, categories. not working for strategic goals and Strateigc Programs.
</commit_message>
<xml_diff>
--- a/data/DummyData.xlsx
+++ b/data/DummyData.xlsx
@@ -507,13 +507,16 @@
         <v>Change.</v>
       </c>
       <c r="F3" t="str">
-        <v>This is a change to the Q1 Objectives to see if it holds.</v>
+        <v>This is a change to the Q1 Objectives to see if it holds. CHANGE</v>
       </c>
       <c r="G3" t="str">
-        <v>change 2.</v>
+        <v>change 2. CHANGE</v>
+      </c>
+      <c r="H3" t="str">
+        <v>CHANGE</v>
       </c>
       <c r="I3" t="str">
-        <v>3</v>
+        <v>CHANGE!@!</v>
       </c>
       <c r="L3" t="str">
         <v>Dr. Alice Nguyen</v>
@@ -531,7 +534,7 @@
         <v>missed</v>
       </c>
       <c r="Q3" t="str">
-        <v>Second phase biomarker validation project building on BD-01 learnings. Focus on protocol standardization and data quality assurance will be essential for regulatory acceptance.</v>
+        <v>Second phase biomarker validation project building on BD-01 learnings. Focus on protocol standardization and data quality assurance will be essential for regulatory acceptance. CHANGE</v>
       </c>
     </row>
     <row r="4">

</xml_diff>